<commit_message>
Update English and Russian data
</commit_message>
<xml_diff>
--- a/Data/source/Russian/Water footprint (Russian).xlsx
+++ b/Data/source/Russian/Water footprint (Russian).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="538">
   <si>
     <t>ID</t>
   </si>
@@ -418,10 +418,7 @@
     <t>Cabbages</t>
   </si>
   <si>
-    <t>Капуста кочанная</t>
-  </si>
-  <si>
-    <t>Белокочанная</t>
+    <t>Капуста белокочанная</t>
   </si>
   <si>
     <t>Cardamoms</t>
@@ -934,7 +931,7 @@
     <t>Olive oil</t>
   </si>
   <si>
-    <t>Оливковое масло рафинированное (refined)</t>
+    <t>Оливковое масло очищенное</t>
   </si>
   <si>
     <t>Palm oil</t>
@@ -1400,9 +1397,6 @@
   </si>
   <si>
     <t>Тыква</t>
-  </si>
-  <si>
-    <t>Squash</t>
   </si>
   <si>
     <t>Melon seed</t>
@@ -2847,9 +2841,7 @@
       <c r="D56" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E56" s="9" t="s">
-        <v>136</v>
-      </c>
+      <c r="E56" s="9"/>
       <c r="F56" s="7">
         <v>280.0</v>
       </c>
@@ -2862,11 +2854,11 @@
         <v>31.0</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F57" s="7">
         <v>34319.0</v>
@@ -2880,14 +2872,14 @@
         <v>168.0</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="F58" s="7">
         <v>287.0</v>
@@ -2901,11 +2893,11 @@
         <v>166.0</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F59" s="7">
         <v>1436.0</v>
@@ -2919,11 +2911,11 @@
         <v>211.0</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F60" s="7">
         <v>1436.0</v>
@@ -2937,11 +2929,11 @@
         <v>165.0</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F61" s="7">
         <v>1044.0</v>
@@ -2955,11 +2947,11 @@
         <v>167.0</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F62" s="7">
         <v>1512.0</v>
@@ -2973,14 +2965,14 @@
         <v>37.0</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E63" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="F63" s="7">
         <v>24740.0</v>
@@ -2994,11 +2986,11 @@
         <v>42.0</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F64" s="7">
         <v>2750.0</v>
@@ -3012,14 +3004,14 @@
         <v>35.0</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E65" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="F65" s="7">
         <v>14218.0</v>
@@ -3033,11 +3025,11 @@
         <v>104.0</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F66" s="7">
         <v>514.0</v>
@@ -3051,11 +3043,11 @@
         <v>49.0</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F67" s="7">
         <v>748.0</v>
@@ -3069,14 +3061,14 @@
         <v>38.0</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F68" s="7">
         <v>9896.0</v>
@@ -3090,11 +3082,11 @@
         <v>70.0</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F69" s="7">
         <v>276.0</v>
@@ -3108,11 +3100,11 @@
         <v>107.0</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F70" s="7">
         <v>17093.0</v>
@@ -3126,13 +3118,13 @@
         <v>86.0</v>
       </c>
       <c r="B71" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="D71" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="F71" s="7">
         <v>5521.0</v>
@@ -3146,16 +3138,16 @@
         <v>55.0</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="D72" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="E72" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="F72" s="7">
         <v>2449.0</v>
@@ -3169,16 +3161,16 @@
         <v>56.0</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="D73" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="E73" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>178</v>
       </c>
       <c r="F73" s="7">
         <v>4490.0</v>
@@ -3192,11 +3184,11 @@
         <v>58.0</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F74" s="7">
         <v>1256.0</v>
@@ -3210,11 +3202,11 @@
         <v>57.0</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F75" s="7">
         <v>2687.0</v>
@@ -3228,11 +3220,11 @@
         <v>105.0</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F76" s="7">
         <v>23391.0</v>
@@ -3246,11 +3238,11 @@
         <v>100.0</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F77" s="7">
         <v>3685.0</v>
@@ -3264,11 +3256,11 @@
         <v>61.0</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F78" s="7">
         <v>2093.0</v>
@@ -3282,11 +3274,11 @@
         <v>62.0</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F79" s="7">
         <v>8280.0</v>
@@ -3300,11 +3292,11 @@
         <v>63.0</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F80" s="7">
         <v>8280.0</v>
@@ -3318,13 +3310,13 @@
         <v>48.0</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="D81" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>193</v>
       </c>
       <c r="F81" s="7">
         <v>15526.0</v>
@@ -3338,14 +3330,14 @@
         <v>69.0</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>196</v>
       </c>
       <c r="F82" s="7">
         <v>6906.0</v>
@@ -3359,11 +3351,11 @@
         <v>59.0</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F83" s="7">
         <v>15897.0</v>
@@ -3377,11 +3369,11 @@
         <v>60.0</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F84" s="7">
         <v>18925.0</v>
@@ -3395,11 +3387,11 @@
         <v>87.0</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F85" s="7">
         <v>526.0</v>
@@ -3413,16 +3405,16 @@
         <v>114.0</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="D86" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="E86" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>206</v>
       </c>
       <c r="F86" s="7">
         <v>1222.0</v>
@@ -3436,13 +3428,13 @@
         <v>119.0</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D87" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>208</v>
       </c>
       <c r="F87" s="7">
         <v>700.0</v>
@@ -3456,16 +3448,16 @@
         <v>116.0</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D88" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C88" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>210</v>
-      </c>
       <c r="E88" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F88" s="7">
         <v>1081.0</v>
@@ -3479,16 +3471,16 @@
         <v>115.0</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D89" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C89" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>212</v>
-      </c>
       <c r="E89" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F89" s="7">
         <v>1253.0</v>
@@ -3502,16 +3494,16 @@
         <v>117.0</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D90" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C90" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D90" s="9" t="s">
-        <v>214</v>
-      </c>
       <c r="E90" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F90" s="7">
         <v>2575.0</v>
@@ -3525,16 +3517,16 @@
         <v>118.0</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D91" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C91" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D91" s="9" t="s">
-        <v>216</v>
-      </c>
       <c r="E91" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F91" s="7">
         <v>1671.0</v>
@@ -3548,14 +3540,14 @@
         <v>183.0</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E92" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="F92" s="7">
         <v>21793.0</v>
@@ -3569,11 +3561,11 @@
         <v>184.0</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F93" s="7">
         <v>9371.0</v>
@@ -3587,14 +3579,14 @@
         <v>44.0</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E94" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>224</v>
       </c>
       <c r="F94" s="7">
         <v>4325.0</v>
@@ -3608,14 +3600,14 @@
         <v>88.0</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>227</v>
       </c>
       <c r="F95" s="7">
         <v>336.0</v>
@@ -3629,11 +3621,11 @@
         <v>111.0</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F96" s="7">
         <v>642.0</v>
@@ -3647,11 +3639,11 @@
         <v>110.0</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F97" s="7">
         <v>237.0</v>
@@ -3665,11 +3657,11 @@
         <v>108.0</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F98" s="7">
         <v>642.0</v>
@@ -3683,11 +3675,11 @@
         <v>113.0</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F99" s="7">
         <v>9415.0</v>
@@ -3701,11 +3693,11 @@
         <v>80.0</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E100" s="9"/>
       <c r="F100" s="7">
@@ -3720,11 +3712,11 @@
         <v>112.0</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F101" s="7">
         <v>5168.0</v>
@@ -3738,11 +3730,11 @@
         <v>163.0</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F102" s="7">
         <v>2188.0</v>
@@ -3756,14 +3748,14 @@
         <v>75.0</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E103" s="9" t="s">
         <v>243</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="F103" s="7">
         <v>1849.0</v>
@@ -3777,11 +3769,11 @@
         <v>173.0</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F104" s="7">
         <v>413.0</v>
@@ -3795,11 +3787,11 @@
         <v>123.0</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F105" s="7">
         <v>1800.0</v>
@@ -3813,14 +3805,14 @@
         <v>124.0</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E106" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>251</v>
       </c>
       <c r="F106" s="7">
         <v>1800.0</v>
@@ -3834,11 +3826,11 @@
         <v>122.0</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F107" s="7">
         <v>748.0</v>
@@ -3852,13 +3844,13 @@
         <v>125.0</v>
       </c>
       <c r="B108" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="D108" s="9" t="s">
         <v>255</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>256</v>
       </c>
       <c r="F108" s="7">
         <v>20388.0</v>
@@ -3872,16 +3864,16 @@
         <v>126.0</v>
       </c>
       <c r="B109" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="D109" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="D109" s="9" t="s">
+      <c r="E109" s="9" t="s">
         <v>259</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>260</v>
       </c>
       <c r="F109" s="7">
         <v>564.0</v>
@@ -3895,14 +3887,14 @@
         <v>74.0</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>263</v>
       </c>
       <c r="F110" s="7">
         <v>1610.0</v>
@@ -3916,16 +3908,16 @@
         <v>127.0</v>
       </c>
       <c r="B111" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D111" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>265</v>
-      </c>
       <c r="E111" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F111" s="7">
         <v>2254.0</v>
@@ -3939,14 +3931,14 @@
         <v>36.0</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F112" s="7">
         <v>1878.0</v>
@@ -3960,14 +3952,14 @@
         <v>210.0</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C113" s="8"/>
       <c r="D113" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F113" s="7">
         <v>2818.0</v>
@@ -3981,14 +3973,14 @@
         <v>139.0</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C114" s="8"/>
       <c r="D114" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E114" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>272</v>
       </c>
       <c r="F114" s="7">
         <v>1098.0</v>
@@ -4002,7 +3994,7 @@
         <v>28.0</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="9" t="s">
@@ -4020,11 +4012,11 @@
         <v>3.0</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C116" s="8"/>
       <c r="D116" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F116" s="7">
         <v>16095.0</v>
@@ -4038,11 +4030,11 @@
         <v>4.0</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C117" s="8"/>
       <c r="D117" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F117" s="7">
         <v>8047.0</v>
@@ -4056,11 +4048,11 @@
         <v>129.0</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C118" s="8"/>
       <c r="D118" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F118" s="7">
         <v>1020.0</v>
@@ -4074,11 +4066,11 @@
         <v>130.0</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F119" s="7">
         <v>4745.0</v>
@@ -4092,11 +4084,11 @@
         <v>33.0</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C120" s="8"/>
       <c r="D120" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F120" s="7">
         <v>195.0</v>
@@ -4110,13 +4102,13 @@
         <v>135.0</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="D121" s="9" t="s">
         <v>285</v>
-      </c>
-      <c r="D121" s="9" t="s">
-        <v>286</v>
       </c>
       <c r="F121" s="7">
         <v>34319.0</v>
@@ -4130,11 +4122,11 @@
         <v>156.0</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F122" s="7">
         <v>288.0</v>
@@ -4148,11 +4140,11 @@
         <v>134.0</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F123" s="7">
         <v>910.0</v>
@@ -4166,14 +4158,14 @@
         <v>43.0</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C124" s="8"/>
       <c r="D124" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E124" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="E124" s="9" t="s">
-        <v>293</v>
       </c>
       <c r="F124" s="7">
         <v>4177.0</v>
@@ -4187,11 +4179,11 @@
         <v>137.0</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C125" s="8"/>
       <c r="D125" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F125" s="7">
         <v>1788.0</v>
@@ -4205,11 +4197,11 @@
         <v>136.0</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C126" s="8"/>
       <c r="D126" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F126" s="7">
         <v>2536.0</v>
@@ -4223,11 +4215,11 @@
         <v>138.0</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C127" s="8"/>
       <c r="D127" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F127" s="7">
         <v>2416.0</v>
@@ -4241,11 +4233,11 @@
         <v>71.0</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C128" s="8"/>
       <c r="D128" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F128" s="7">
         <v>353.0</v>
@@ -4259,11 +4251,11 @@
         <v>143.0</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F129" s="7">
         <v>3015.0</v>
@@ -4277,11 +4269,11 @@
         <v>142.0</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C130" s="8"/>
       <c r="D130" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F130" s="7">
         <v>14431.0</v>
@@ -4295,11 +4287,11 @@
         <v>141.0</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C131" s="8"/>
       <c r="D131" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F131" s="7">
         <v>14726.0</v>
@@ -4313,11 +4305,11 @@
         <v>150.0</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C132" s="8"/>
       <c r="D132" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F132" s="7">
         <v>4971.0</v>
@@ -4331,11 +4323,11 @@
         <v>149.0</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C133" s="8"/>
       <c r="D133" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F133" s="7">
         <v>2868.0</v>
@@ -4349,13 +4341,13 @@
         <v>148.0</v>
       </c>
       <c r="B134" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C134" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="C134" s="8" t="s">
+      <c r="D134" s="9" t="s">
         <v>313</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>314</v>
       </c>
       <c r="F134" s="7">
         <v>5401.0</v>
@@ -4369,14 +4361,14 @@
         <v>151.0</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E135" s="9" t="s">
         <v>316</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>317</v>
       </c>
       <c r="F135" s="7">
         <v>460.0</v>
@@ -4390,11 +4382,11 @@
         <v>99.0</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F136" s="7">
         <v>2447.0</v>
@@ -4408,14 +4400,14 @@
         <v>45.0</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C137" s="8"/>
       <c r="D137" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E137" s="9" t="s">
         <v>321</v>
-      </c>
-      <c r="E137" s="9" t="s">
-        <v>322</v>
       </c>
       <c r="F137" s="7">
         <v>7365.0</v>
@@ -4429,14 +4421,14 @@
         <v>46.0</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F138" s="7">
         <v>379.0</v>
@@ -4450,11 +4442,11 @@
         <v>152.0</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C139" s="8"/>
       <c r="D139" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F139" s="7">
         <v>910.0</v>
@@ -4468,11 +4460,11 @@
         <v>21.0</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C140" s="8"/>
       <c r="D140" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F140" s="7">
         <v>298.0</v>
@@ -4486,14 +4478,14 @@
         <v>161.0</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C141" s="8"/>
       <c r="D141" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="E141" s="9" t="s">
         <v>330</v>
-      </c>
-      <c r="E141" s="9" t="s">
-        <v>331</v>
       </c>
       <c r="F141" s="7">
         <v>1602.0</v>
@@ -4507,14 +4499,14 @@
         <v>207.0</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C142" s="8"/>
       <c r="D142" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="E142" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="E142" s="9" t="s">
-        <v>334</v>
       </c>
       <c r="F142" s="7">
         <v>3366.0</v>
@@ -4528,11 +4520,11 @@
         <v>206.0</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F143" s="7">
         <v>6792.0</v>
@@ -4546,11 +4538,11 @@
         <v>228.0</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C144" s="8"/>
       <c r="D144" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F144" s="7">
         <v>1827.0</v>
@@ -4564,14 +4556,14 @@
         <v>230.0</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C145" s="8"/>
       <c r="D145" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="E145" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="E145" s="9" t="s">
-        <v>341</v>
       </c>
       <c r="F145" s="7">
         <v>4189.0</v>
@@ -4585,11 +4577,11 @@
         <v>229.0</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C146" s="8"/>
       <c r="D146" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F146" s="7">
         <v>1849.0</v>
@@ -4603,11 +4595,11 @@
         <v>231.0</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C147" s="8"/>
       <c r="D147" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F147" s="7">
         <v>2036.0</v>
@@ -4621,11 +4613,11 @@
         <v>232.0</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F148" s="7">
         <v>1436.0</v>
@@ -4639,11 +4631,11 @@
         <v>131.0</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C149" s="8"/>
       <c r="D149" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F149" s="7">
         <v>4478.0</v>
@@ -4657,14 +4649,14 @@
         <v>170.0</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="E150" s="9" t="s">
         <v>351</v>
-      </c>
-      <c r="E150" s="9" t="s">
-        <v>352</v>
       </c>
       <c r="F150" s="7">
         <v>4507.0</v>
@@ -4678,11 +4670,11 @@
         <v>172.0</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F151" s="7">
         <v>2271.0</v>
@@ -4696,11 +4688,11 @@
         <v>171.0</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C152" s="8"/>
       <c r="D152" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F152" s="7">
         <v>4301.0</v>
@@ -4714,14 +4706,14 @@
         <v>133.0</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C153" s="8"/>
       <c r="D153" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="E153" s="9" t="s">
         <v>358</v>
-      </c>
-      <c r="E153" s="9" t="s">
-        <v>359</v>
       </c>
       <c r="F153" s="7">
         <v>13748.0</v>
@@ -4735,11 +4727,11 @@
         <v>180.0</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F154" s="7">
         <v>1930.0</v>
@@ -4753,11 +4745,11 @@
         <v>176.0</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F155" s="7">
         <v>2497.0</v>
@@ -4771,13 +4763,13 @@
         <v>177.0</v>
       </c>
       <c r="B156" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C156" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="C156" s="8" t="s">
+      <c r="D156" s="9" t="s">
         <v>365</v>
-      </c>
-      <c r="D156" s="9" t="s">
-        <v>366</v>
       </c>
       <c r="F156" s="7">
         <v>2172.0</v>
@@ -4791,11 +4783,11 @@
         <v>178.0</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F157" s="7">
         <v>1673.0</v>
@@ -4809,11 +4801,11 @@
         <v>174.0</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F158" s="7">
         <v>2230.0</v>
@@ -4827,11 +4819,11 @@
         <v>175.0</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F159" s="7">
         <v>2628.0</v>
@@ -4845,11 +4837,11 @@
         <v>32.0</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C160" s="8"/>
       <c r="D160" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F160" s="7">
         <v>5594.0</v>
@@ -4863,11 +4855,11 @@
         <v>179.0</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C161" s="8"/>
       <c r="D161" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F161" s="7">
         <v>1544.0</v>
@@ -4881,14 +4873,14 @@
         <v>181.0</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C162" s="8"/>
       <c r="D162" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="E162" s="9" t="s">
         <v>378</v>
-      </c>
-      <c r="E162" s="9" t="s">
-        <v>379</v>
       </c>
       <c r="F162" s="7">
         <v>7221.0</v>
@@ -4902,14 +4894,14 @@
         <v>205.0</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E163" s="9" t="s">
         <v>381</v>
-      </c>
-      <c r="E163" s="9" t="s">
-        <v>382</v>
       </c>
       <c r="F163" s="7">
         <v>1782.0</v>
@@ -4923,11 +4915,11 @@
         <v>203.0</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F164" s="7">
         <v>865.0</v>
@@ -4941,11 +4933,11 @@
         <v>204.0</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C165" s="8"/>
       <c r="D165" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F165" s="7">
         <v>1666.0</v>
@@ -4959,11 +4951,11 @@
         <v>201.0</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C166" s="8"/>
       <c r="D166" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F166" s="7">
         <v>132.0</v>
@@ -4977,11 +4969,11 @@
         <v>202.0</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F167" s="7">
         <v>210.0</v>
@@ -4995,16 +4987,16 @@
         <v>164.0</v>
       </c>
       <c r="B168" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C168" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="C168" s="8" t="s">
+      <c r="D168" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D168" s="9" t="s">
+      <c r="E168" s="9" t="s">
         <v>393</v>
-      </c>
-      <c r="E168" s="9" t="s">
-        <v>394</v>
       </c>
       <c r="F168" s="7">
         <v>5988.0</v>
@@ -5018,11 +5010,11 @@
         <v>186.0</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C169" s="8"/>
       <c r="D169" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F169" s="7">
         <v>7824.0</v>
@@ -5036,14 +5028,14 @@
         <v>185.0</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C170" s="8"/>
       <c r="D170" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="E170" s="9" t="s">
         <v>398</v>
-      </c>
-      <c r="E170" s="9" t="s">
-        <v>399</v>
       </c>
       <c r="F170" s="7">
         <v>7041.0</v>
@@ -5057,11 +5049,11 @@
         <v>162.0</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F171" s="7">
         <v>2180.0</v>
@@ -5075,14 +5067,14 @@
         <v>72.0</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C172" s="8"/>
       <c r="D172" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E172" s="9" t="s">
         <v>403</v>
-      </c>
-      <c r="E172" s="9" t="s">
-        <v>404</v>
       </c>
       <c r="F172" s="7">
         <v>499.0</v>
@@ -5096,11 +5088,11 @@
         <v>192.0</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C173" s="8"/>
       <c r="D173" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F173" s="7">
         <v>2145.0</v>
@@ -5114,11 +5106,11 @@
         <v>194.0</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C174" s="8"/>
       <c r="D174" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F174" s="7">
         <v>572.0</v>
@@ -5132,11 +5124,11 @@
         <v>196.0</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C175" s="8"/>
       <c r="D175" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F175" s="7">
         <v>4190.0</v>
@@ -5150,11 +5142,11 @@
         <v>190.0</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C176" s="8"/>
       <c r="D176" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F176" s="7">
         <v>3763.0</v>
@@ -5168,11 +5160,11 @@
         <v>195.0</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C177" s="8"/>
       <c r="D177" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F177" s="7">
         <v>613.0</v>
@@ -5186,11 +5178,11 @@
         <v>121.0</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F178" s="7">
         <v>2437.0</v>
@@ -5204,11 +5196,11 @@
         <v>120.0</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C179" s="8"/>
       <c r="D179" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F179" s="7">
         <v>1950.0</v>
@@ -5222,11 +5214,11 @@
         <v>84.0</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C180" s="8"/>
       <c r="D180" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F180" s="7">
         <v>353.0</v>
@@ -5240,11 +5232,11 @@
         <v>188.0</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F181" s="7">
         <v>3048.0</v>
@@ -5258,11 +5250,11 @@
         <v>191.0</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F182" s="7">
         <v>2523.0</v>
@@ -5276,11 +5268,11 @@
         <v>12.0</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C183" s="8"/>
       <c r="D183" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F183" s="7">
         <v>2150.0</v>
@@ -5294,11 +5286,11 @@
         <v>40.0</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C184" s="8"/>
       <c r="D184" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F184" s="7">
         <v>5060.0</v>
@@ -5312,11 +5304,11 @@
         <v>214.0</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F185" s="7">
         <v>2925.0</v>
@@ -5330,16 +5322,16 @@
         <v>212.0</v>
       </c>
       <c r="B186" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C186" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="C186" s="8" t="s">
+      <c r="D186" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="D186" s="9" t="s">
+      <c r="E186" s="9" t="s">
         <v>433</v>
-      </c>
-      <c r="E186" s="9" t="s">
-        <v>434</v>
       </c>
       <c r="F186" s="7">
         <v>606.0</v>
@@ -5353,14 +5345,14 @@
         <v>218.0</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C187" s="8"/>
       <c r="D187" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E187" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="E187" s="9" t="s">
-        <v>437</v>
       </c>
       <c r="F187" s="7">
         <v>855.0</v>
@@ -5374,14 +5366,14 @@
         <v>219.0</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C188" s="8"/>
       <c r="D188" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E188" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F188" s="7">
         <v>713.0</v>
@@ -5395,14 +5387,14 @@
         <v>217.0</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E189" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F189" s="7">
         <v>534.0</v>
@@ -5416,14 +5408,14 @@
         <v>215.0</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C190" s="8"/>
       <c r="D190" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E190" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F190" s="7">
         <v>267.0</v>
@@ -5437,14 +5429,14 @@
         <v>216.0</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C191" s="8"/>
       <c r="D191" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E191" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F191" s="7">
         <v>1069.0</v>
@@ -5458,14 +5450,14 @@
         <v>221.0</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E192" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F192" s="7">
         <v>214.0</v>
@@ -5479,14 +5471,14 @@
         <v>220.0</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C193" s="8"/>
       <c r="D193" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E193" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F193" s="7">
         <v>4276.0</v>
@@ -5500,14 +5492,14 @@
         <v>222.0</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C194" s="8"/>
       <c r="D194" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E194" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F194" s="7">
         <v>267.0</v>
@@ -5521,14 +5513,14 @@
         <v>193.0</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C195" s="8"/>
       <c r="D195" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E195" s="9" t="s">
         <v>453</v>
-      </c>
-      <c r="E195" s="9" t="s">
-        <v>454</v>
       </c>
       <c r="F195" s="7">
         <v>2523.0</v>
@@ -5542,14 +5534,14 @@
         <v>30.0</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C196" s="8"/>
       <c r="D196" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E196" s="9" t="s">
         <v>456</v>
-      </c>
-      <c r="E196" s="9" t="s">
-        <v>457</v>
       </c>
       <c r="F196" s="7">
         <v>527.0</v>
@@ -5563,14 +5555,14 @@
         <v>223.0</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C197" s="8"/>
       <c r="D197" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="E197" s="9" t="s">
         <v>459</v>
-      </c>
-      <c r="E197" s="9" t="s">
-        <v>460</v>
       </c>
       <c r="F197" s="7">
         <v>195.0</v>
@@ -5584,11 +5576,11 @@
         <v>169.0</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C198" s="8"/>
       <c r="D198" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F198" s="7">
         <v>336.0</v>
@@ -5599,25 +5591,25 @@
     </row>
     <row r="199">
       <c r="A199" s="7">
-        <v>198.0</v>
+        <v>128.0</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F199" s="7">
-        <v>336.0</v>
+        <v>5184.0</v>
       </c>
       <c r="G199" s="9">
-        <v>198.0</v>
+        <v>199.0</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="7">
-        <v>128.0</v>
+        <v>187.0</v>
       </c>
       <c r="B200" s="7" t="s">
         <v>464</v>
@@ -5626,79 +5618,79 @@
       <c r="D200" s="9" t="s">
         <v>465</v>
       </c>
+      <c r="E200" s="9" t="s">
+        <v>466</v>
+      </c>
       <c r="F200" s="7">
-        <v>5184.0</v>
+        <v>2180.0</v>
       </c>
       <c r="G200" s="9">
-        <v>199.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="7">
-        <v>187.0</v>
+        <v>78.0</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C201" s="8"/>
       <c r="D201" s="9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E201" s="9" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F201" s="7">
-        <v>2180.0</v>
+        <v>8280.0</v>
       </c>
       <c r="G201" s="9">
-        <v>200.0</v>
+        <v>201.0</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="7">
-        <v>78.0</v>
+        <v>73.0</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C202" s="8"/>
       <c r="D202" s="9" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E202" s="9" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F202" s="7">
-        <v>8280.0</v>
+        <v>2277.0</v>
       </c>
       <c r="G202" s="9">
-        <v>201.0</v>
+        <v>202.0</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="7">
-        <v>73.0</v>
+        <v>160.0</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C203" s="8"/>
       <c r="D203" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="E203" s="9" t="s">
         <v>474</v>
       </c>
       <c r="F203" s="7">
-        <v>2277.0</v>
+        <v>11363.0</v>
       </c>
       <c r="G203" s="9">
-        <v>202.0</v>
+        <v>203.0</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="7">
-        <v>160.0</v>
+        <v>81.0</v>
       </c>
       <c r="B204" s="7" t="s">
         <v>475</v>
@@ -5708,15 +5700,15 @@
         <v>476</v>
       </c>
       <c r="F204" s="7">
-        <v>11363.0</v>
+        <v>1782.0</v>
       </c>
       <c r="G204" s="9">
-        <v>203.0</v>
+        <v>204.0</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="7">
-        <v>81.0</v>
+        <v>98.0</v>
       </c>
       <c r="B205" s="7" t="s">
         <v>477</v>
@@ -5725,37 +5717,40 @@
       <c r="D205" s="9" t="s">
         <v>478</v>
       </c>
+      <c r="E205" s="9" t="s">
+        <v>479</v>
+      </c>
       <c r="F205" s="7">
-        <v>1782.0</v>
+        <v>5258.0</v>
       </c>
       <c r="G205" s="9">
-        <v>204.0</v>
+        <v>205.0</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="7">
-        <v>98.0</v>
+        <v>97.0</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="9" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E206" s="9" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F206" s="7">
-        <v>5258.0</v>
+        <v>10515.0</v>
       </c>
       <c r="G206" s="9">
-        <v>205.0</v>
+        <v>206.0</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="7">
-        <v>97.0</v>
+        <v>23.0</v>
       </c>
       <c r="B207" s="7" t="s">
         <v>482</v>
@@ -5764,19 +5759,16 @@
       <c r="D207" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="E207" s="9" t="s">
-        <v>481</v>
-      </c>
       <c r="F207" s="7">
-        <v>10515.0</v>
+        <v>1608.0</v>
       </c>
       <c r="G207" s="9">
-        <v>206.0</v>
+        <v>207.0</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="7">
-        <v>23.0</v>
+        <v>68.0</v>
       </c>
       <c r="B208" s="7" t="s">
         <v>484</v>
@@ -5785,37 +5777,37 @@
       <c r="D208" s="9" t="s">
         <v>485</v>
       </c>
+      <c r="E208" s="9" t="s">
+        <v>486</v>
+      </c>
       <c r="F208" s="7">
-        <v>1608.0</v>
+        <v>3957.0</v>
       </c>
       <c r="G208" s="9">
-        <v>207.0</v>
+        <v>208.0</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="7">
-        <v>68.0</v>
+        <v>182.0</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C209" s="8"/>
       <c r="D209" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="E209" s="9" t="s">
         <v>488</v>
       </c>
       <c r="F209" s="7">
-        <v>3957.0</v>
+        <v>4029.0</v>
       </c>
       <c r="G209" s="9">
-        <v>208.0</v>
+        <v>209.0</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="7">
-        <v>182.0</v>
+        <v>67.0</v>
       </c>
       <c r="B210" s="7" t="s">
         <v>489</v>
@@ -5825,15 +5817,15 @@
         <v>490</v>
       </c>
       <c r="F210" s="7">
-        <v>4029.0</v>
+        <v>1332.0</v>
       </c>
       <c r="G210" s="9">
-        <v>209.0</v>
+        <v>210.0</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="7">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="B211" s="7" t="s">
         <v>491</v>
@@ -5843,15 +5835,15 @@
         <v>492</v>
       </c>
       <c r="F211" s="7">
-        <v>1332.0</v>
+        <v>9982.0</v>
       </c>
       <c r="G211" s="9">
-        <v>210.0</v>
+        <v>211.0</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="7">
-        <v>64.0</v>
+        <v>101.0</v>
       </c>
       <c r="B212" s="7" t="s">
         <v>493</v>
@@ -5861,15 +5853,15 @@
         <v>494</v>
       </c>
       <c r="F212" s="7">
-        <v>9982.0</v>
+        <v>4065.0</v>
       </c>
       <c r="G212" s="9">
-        <v>211.0</v>
+        <v>212.0</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="7">
-        <v>101.0</v>
+        <v>102.0</v>
       </c>
       <c r="B213" s="7" t="s">
         <v>495</v>
@@ -5879,15 +5871,15 @@
         <v>496</v>
       </c>
       <c r="F213" s="7">
-        <v>4065.0</v>
+        <v>16259.0</v>
       </c>
       <c r="G213" s="9">
-        <v>212.0</v>
+        <v>213.0</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="7">
-        <v>102.0</v>
+        <v>39.0</v>
       </c>
       <c r="B214" s="7" t="s">
         <v>497</v>
@@ -5897,15 +5889,15 @@
         <v>498</v>
       </c>
       <c r="F214" s="7">
-        <v>16259.0</v>
+        <v>285.0</v>
       </c>
       <c r="G214" s="9">
-        <v>213.0</v>
+        <v>214.0</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="7">
-        <v>39.0</v>
+        <v>213.0</v>
       </c>
       <c r="B215" s="7" t="s">
         <v>499</v>
@@ -5915,15 +5907,15 @@
         <v>500</v>
       </c>
       <c r="F215" s="7">
-        <v>285.0</v>
+        <v>8856.0</v>
       </c>
       <c r="G215" s="9">
-        <v>214.0</v>
+        <v>215.0</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="7">
-        <v>213.0</v>
+        <v>41.0</v>
       </c>
       <c r="B216" s="7" t="s">
         <v>501</v>
@@ -5932,37 +5924,37 @@
       <c r="D216" s="9" t="s">
         <v>502</v>
       </c>
+      <c r="E216" s="9" t="s">
+        <v>503</v>
+      </c>
       <c r="F216" s="7">
-        <v>8856.0</v>
+        <v>1604.0</v>
       </c>
       <c r="G216" s="9">
-        <v>215.0</v>
+        <v>216.0</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="7">
-        <v>41.0</v>
+        <v>22.0</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C217" s="8"/>
       <c r="D217" s="9" t="s">
-        <v>504</v>
-      </c>
-      <c r="E217" s="9" t="s">
         <v>505</v>
       </c>
       <c r="F217" s="7">
-        <v>1604.0</v>
+        <v>845.0</v>
       </c>
       <c r="G217" s="9">
-        <v>216.0</v>
+        <v>217.0</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="7">
-        <v>22.0</v>
+        <v>82.0</v>
       </c>
       <c r="B218" s="7" t="s">
         <v>506</v>
@@ -5972,56 +5964,56 @@
         <v>507</v>
       </c>
       <c r="F218" s="7">
-        <v>845.0</v>
+        <v>589.0</v>
       </c>
       <c r="G218" s="9">
-        <v>217.0</v>
+        <v>218.0</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="7">
-        <v>82.0</v>
+        <v>145.0</v>
       </c>
       <c r="B219" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="C219" s="8"/>
+      <c r="C219" s="8" t="s">
+        <v>509</v>
+      </c>
       <c r="D219" s="9" t="s">
-        <v>509</v>
+        <v>510</v>
+      </c>
+      <c r="E219" s="9" t="s">
+        <v>511</v>
       </c>
       <c r="F219" s="7">
-        <v>589.0</v>
+        <v>272.0</v>
       </c>
       <c r="G219" s="9">
-        <v>218.0</v>
+        <v>219.0</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="7">
-        <v>145.0</v>
+        <v>144.0</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="C220" s="8" t="s">
-        <v>511</v>
-      </c>
+        <v>512</v>
+      </c>
+      <c r="C220" s="8"/>
       <c r="D220" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="E220" s="9" t="s">
         <v>513</v>
       </c>
       <c r="F220" s="7">
-        <v>272.0</v>
+        <v>345.0</v>
       </c>
       <c r="G220" s="9">
-        <v>219.0</v>
+        <v>220.0</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="7">
-        <v>144.0</v>
+        <v>83.0</v>
       </c>
       <c r="B221" s="7" t="s">
         <v>514</v>
@@ -6031,15 +6023,15 @@
         <v>515</v>
       </c>
       <c r="F221" s="7">
-        <v>345.0</v>
+        <v>2265.0</v>
       </c>
       <c r="G221" s="9">
-        <v>220.0</v>
+        <v>221.0</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="7">
-        <v>83.0</v>
+        <v>109.0</v>
       </c>
       <c r="B222" s="7" t="s">
         <v>516</v>
@@ -6049,15 +6041,15 @@
         <v>517</v>
       </c>
       <c r="F222" s="7">
-        <v>2265.0</v>
+        <v>5874.0</v>
       </c>
       <c r="G222" s="9">
-        <v>221.0</v>
+        <v>222.0</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="7">
-        <v>109.0</v>
+        <v>47.0</v>
       </c>
       <c r="B223" s="7" t="s">
         <v>518</v>
@@ -6067,15 +6059,15 @@
         <v>519</v>
       </c>
       <c r="F223" s="7">
-        <v>5874.0</v>
+        <v>17196.0</v>
       </c>
       <c r="G223" s="9">
-        <v>222.0</v>
+        <v>223.0</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="7">
-        <v>47.0</v>
+        <v>197.0</v>
       </c>
       <c r="B224" s="7" t="s">
         <v>520</v>
@@ -6085,15 +6077,15 @@
         <v>521</v>
       </c>
       <c r="F224" s="7">
-        <v>17196.0</v>
+        <v>292.0</v>
       </c>
       <c r="G224" s="9">
-        <v>223.0</v>
+        <v>224.0</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="7">
-        <v>197.0</v>
+        <v>34.0</v>
       </c>
       <c r="B225" s="7" t="s">
         <v>522</v>
@@ -6103,15 +6095,15 @@
         <v>523</v>
       </c>
       <c r="F225" s="7">
-        <v>292.0</v>
+        <v>3793.0</v>
       </c>
       <c r="G225" s="9">
-        <v>224.0</v>
+        <v>225.0</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="7">
-        <v>34.0</v>
+        <v>8.0</v>
       </c>
       <c r="B226" s="7" t="s">
         <v>524</v>
@@ -6121,15 +6113,15 @@
         <v>525</v>
       </c>
       <c r="F226" s="7">
-        <v>3793.0</v>
+        <v>822.0</v>
       </c>
       <c r="G226" s="9">
-        <v>225.0</v>
+        <v>226.0</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="7">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B227" s="7" t="s">
         <v>526</v>
@@ -6139,15 +6131,15 @@
         <v>527</v>
       </c>
       <c r="F227" s="7">
-        <v>822.0</v>
+        <v>6847.0</v>
       </c>
       <c r="G227" s="9">
-        <v>226.0</v>
+        <v>227.0</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="7">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B228" s="7" t="s">
         <v>528</v>
@@ -6157,15 +6149,15 @@
         <v>529</v>
       </c>
       <c r="F228" s="7">
-        <v>6847.0</v>
+        <v>1141.0</v>
       </c>
       <c r="G228" s="9">
-        <v>227.0</v>
+        <v>228.0</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="7">
-        <v>6.0</v>
+        <v>76.0</v>
       </c>
       <c r="B229" s="7" t="s">
         <v>530</v>
@@ -6175,15 +6167,15 @@
         <v>531</v>
       </c>
       <c r="F229" s="7">
-        <v>1141.0</v>
+        <v>3265.0</v>
       </c>
       <c r="G229" s="9">
-        <v>228.0</v>
+        <v>229.0</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="7">
-        <v>76.0</v>
+        <v>234.0</v>
       </c>
       <c r="B230" s="7" t="s">
         <v>532</v>
@@ -6193,15 +6185,15 @@
         <v>533</v>
       </c>
       <c r="F230" s="7">
-        <v>3265.0</v>
+        <v>343.0</v>
       </c>
       <c r="G230" s="9">
-        <v>229.0</v>
+        <v>230.0</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="7">
-        <v>234.0</v>
+        <v>17.0</v>
       </c>
       <c r="B231" s="7" t="s">
         <v>534</v>
@@ -6211,15 +6203,15 @@
         <v>535</v>
       </c>
       <c r="F231" s="7">
-        <v>343.0</v>
+        <v>1977.0</v>
       </c>
       <c r="G231" s="9">
-        <v>230.0</v>
+        <v>231.0</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="7">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="B232" s="7" t="s">
         <v>536</v>
@@ -6229,29 +6221,15 @@
         <v>537</v>
       </c>
       <c r="F232" s="7">
-        <v>1977.0</v>
+        <v>1423.0</v>
       </c>
       <c r="G232" s="9">
-        <v>231.0</v>
+        <v>232.0</v>
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="7">
-        <v>16.0</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="C233" s="8"/>
-      <c r="D233" s="9" t="s">
-        <v>539</v>
-      </c>
-      <c r="F233" s="7">
-        <v>1423.0</v>
-      </c>
-      <c r="G233" s="9">
-        <v>232.0</v>
-      </c>
+      <c r="C233" s="11"/>
+      <c r="F233" s="12"/>
     </row>
     <row r="234">
       <c r="C234" s="11"/>
@@ -9300,10 +9278,6 @@
     <row r="995">
       <c r="C995" s="11"/>
       <c r="F995" s="12"/>
-    </row>
-    <row r="996">
-      <c r="C996" s="11"/>
-      <c r="F996" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>